<commit_message>
resize images to 600x600 and update annotations
</commit_message>
<xml_diff>
--- a/JDGroup/train_excel.xlsx
+++ b/JDGroup/train_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicapham/Desktop/SeniorDesign/JDGroup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18BE859-4707-054C-BCE9-23EEE8D50678}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04CBA00-EA5C-5E49-8849-0F4A371E3B16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="-300" windowWidth="19020" windowHeight="16280" xr2:uid="{03875F19-7B96-D946-BA10-8A2334F19B5C}"/>
+    <workbookView xWindow="-21600" yWindow="-300" windowWidth="19020" windowHeight="16280" activeTab="1" xr2:uid="{03875F19-7B96-D946-BA10-8A2334F19B5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" r:id="rId1"/>
@@ -1792,8 +1792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9067D9EB-C6F0-0D4F-BA95-5D4A9EAA8C8A}">
   <dimension ref="A1:G242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1839,10 +1839,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F2" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
@@ -1862,10 +1862,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F3" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>1</v>
@@ -1885,10 +1885,10 @@
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F4" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>1</v>
@@ -1908,10 +1908,10 @@
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F5" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>1</v>
@@ -1931,10 +1931,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F6" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
@@ -1954,10 +1954,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F7" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>1</v>
@@ -1977,10 +1977,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F8" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>1</v>
@@ -2000,10 +2000,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F9" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>1</v>
@@ -2023,10 +2023,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F10" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>1</v>
@@ -2046,10 +2046,10 @@
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F11" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>1</v>
@@ -2069,10 +2069,10 @@
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F12" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>1</v>
@@ -2092,10 +2092,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F13" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>1</v>
@@ -2115,10 +2115,10 @@
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F14" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>1</v>
@@ -2138,10 +2138,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F15" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>1</v>
@@ -2161,10 +2161,10 @@
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F16" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>1</v>
@@ -2184,10 +2184,10 @@
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F17" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>1</v>
@@ -2207,10 +2207,10 @@
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F18" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>1</v>
@@ -2230,10 +2230,10 @@
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F19" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>1</v>
@@ -2253,10 +2253,10 @@
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F20" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>1</v>
@@ -2276,10 +2276,10 @@
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F21" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>1</v>
@@ -2299,10 +2299,10 @@
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F22" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>1</v>
@@ -2322,10 +2322,10 @@
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F23" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>1</v>
@@ -2345,10 +2345,10 @@
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F24" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>1</v>
@@ -2368,10 +2368,10 @@
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F25" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>1</v>
@@ -2391,10 +2391,10 @@
         <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F26" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>1</v>
@@ -2414,10 +2414,10 @@
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F27" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>1</v>
@@ -2437,10 +2437,10 @@
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F28" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>1</v>
@@ -2460,10 +2460,10 @@
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F29" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>1</v>
@@ -2483,10 +2483,10 @@
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F30" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>1</v>
@@ -2506,10 +2506,10 @@
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F31" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>1</v>
@@ -2529,10 +2529,10 @@
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F32" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>1</v>
@@ -2552,10 +2552,10 @@
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F33" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>1</v>
@@ -2575,10 +2575,10 @@
         <v>0</v>
       </c>
       <c r="E34" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F34" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>1</v>
@@ -2598,10 +2598,10 @@
         <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F35" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>1</v>
@@ -2621,10 +2621,10 @@
         <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F36" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>1</v>
@@ -2644,10 +2644,10 @@
         <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F37" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>1</v>
@@ -2667,10 +2667,10 @@
         <v>0</v>
       </c>
       <c r="E38" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F38" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>1</v>
@@ -2690,10 +2690,10 @@
         <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F39" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>1</v>
@@ -2713,10 +2713,10 @@
         <v>0</v>
       </c>
       <c r="E40" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F40" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>1</v>
@@ -2736,10 +2736,10 @@
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F41" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>1</v>
@@ -2759,10 +2759,10 @@
         <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F42" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>1</v>
@@ -2782,10 +2782,10 @@
         <v>0</v>
       </c>
       <c r="E43" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F43" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>1</v>
@@ -2805,10 +2805,10 @@
         <v>0</v>
       </c>
       <c r="E44" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F44" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>1</v>
@@ -2828,10 +2828,10 @@
         <v>0</v>
       </c>
       <c r="E45" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F45" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>1</v>
@@ -2851,10 +2851,10 @@
         <v>0</v>
       </c>
       <c r="E46" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F46" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>1</v>
@@ -2874,10 +2874,10 @@
         <v>0</v>
       </c>
       <c r="E47" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F47" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>1</v>
@@ -2897,10 +2897,10 @@
         <v>0</v>
       </c>
       <c r="E48" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F48" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>1</v>
@@ -2920,10 +2920,10 @@
         <v>0</v>
       </c>
       <c r="E49" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F49" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>1</v>
@@ -2943,10 +2943,10 @@
         <v>0</v>
       </c>
       <c r="E50" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F50" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>1</v>
@@ -2966,10 +2966,10 @@
         <v>0</v>
       </c>
       <c r="E51" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F51" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>1</v>
@@ -2989,10 +2989,10 @@
         <v>0</v>
       </c>
       <c r="E52" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F52" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>1</v>
@@ -3012,10 +3012,10 @@
         <v>0</v>
       </c>
       <c r="E53" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F53" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>1</v>
@@ -3035,10 +3035,10 @@
         <v>0</v>
       </c>
       <c r="E54" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F54" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>1</v>
@@ -3058,10 +3058,10 @@
         <v>0</v>
       </c>
       <c r="E55" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F55" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>1</v>
@@ -3081,10 +3081,10 @@
         <v>0</v>
       </c>
       <c r="E56" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F56" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>1</v>
@@ -3104,10 +3104,10 @@
         <v>0</v>
       </c>
       <c r="E57" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F57" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>1</v>
@@ -3127,10 +3127,10 @@
         <v>0</v>
       </c>
       <c r="E58" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F58" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>1</v>
@@ -3150,10 +3150,10 @@
         <v>0</v>
       </c>
       <c r="E59" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F59" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>1</v>
@@ -3173,10 +3173,10 @@
         <v>0</v>
       </c>
       <c r="E60" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F60" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>1</v>
@@ -3196,10 +3196,10 @@
         <v>0</v>
       </c>
       <c r="E61" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F61" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>1</v>
@@ -3219,10 +3219,10 @@
         <v>0</v>
       </c>
       <c r="E62" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F62" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>1</v>
@@ -3242,10 +3242,10 @@
         <v>0</v>
       </c>
       <c r="E63" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F63" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>1</v>
@@ -3265,10 +3265,10 @@
         <v>0</v>
       </c>
       <c r="E64" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F64" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>1</v>
@@ -3288,10 +3288,10 @@
         <v>0</v>
       </c>
       <c r="E65" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F65" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>1</v>
@@ -3311,10 +3311,10 @@
         <v>0</v>
       </c>
       <c r="E66" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F66" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>1</v>
@@ -3334,10 +3334,10 @@
         <v>0</v>
       </c>
       <c r="E67" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F67" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>1</v>
@@ -3357,10 +3357,10 @@
         <v>0</v>
       </c>
       <c r="E68" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F68" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>1</v>
@@ -3380,10 +3380,10 @@
         <v>0</v>
       </c>
       <c r="E69" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F69" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>1</v>
@@ -3403,10 +3403,10 @@
         <v>0</v>
       </c>
       <c r="E70" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F70" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>1</v>
@@ -3426,10 +3426,10 @@
         <v>0</v>
       </c>
       <c r="E71" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F71" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>1</v>
@@ -3449,10 +3449,10 @@
         <v>0</v>
       </c>
       <c r="E72" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F72" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>1</v>
@@ -3472,10 +3472,10 @@
         <v>0</v>
       </c>
       <c r="E73" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F73" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>1</v>
@@ -3495,10 +3495,10 @@
         <v>0</v>
       </c>
       <c r="E74" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F74" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>1</v>
@@ -3518,10 +3518,10 @@
         <v>0</v>
       </c>
       <c r="E75" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F75" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>1</v>
@@ -3541,10 +3541,10 @@
         <v>0</v>
       </c>
       <c r="E76" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F76" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>1</v>
@@ -3564,10 +3564,10 @@
         <v>0</v>
       </c>
       <c r="E77" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F77" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>1</v>
@@ -3587,10 +3587,10 @@
         <v>0</v>
       </c>
       <c r="E78" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F78" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>1</v>
@@ -3610,10 +3610,10 @@
         <v>0</v>
       </c>
       <c r="E79" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F79" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>1</v>
@@ -3633,10 +3633,10 @@
         <v>0</v>
       </c>
       <c r="E80" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F80" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>1</v>
@@ -3656,10 +3656,10 @@
         <v>0</v>
       </c>
       <c r="E81" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F81" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>1</v>
@@ -3679,10 +3679,10 @@
         <v>0</v>
       </c>
       <c r="E82" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F82" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>1</v>
@@ -3702,10 +3702,10 @@
         <v>0</v>
       </c>
       <c r="E83" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F83" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>1</v>
@@ -3725,10 +3725,10 @@
         <v>0</v>
       </c>
       <c r="E84" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F84" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>1</v>
@@ -3748,10 +3748,10 @@
         <v>0</v>
       </c>
       <c r="E85" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F85" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>1</v>
@@ -3771,10 +3771,10 @@
         <v>0</v>
       </c>
       <c r="E86" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F86" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>1</v>
@@ -3794,10 +3794,10 @@
         <v>0</v>
       </c>
       <c r="E87" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F87" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>1</v>
@@ -3817,10 +3817,10 @@
         <v>0</v>
       </c>
       <c r="E88" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F88" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>1</v>
@@ -3840,10 +3840,10 @@
         <v>0</v>
       </c>
       <c r="E89" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F89" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>1</v>
@@ -3863,10 +3863,10 @@
         <v>0</v>
       </c>
       <c r="E90" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F90" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>1</v>
@@ -3886,10 +3886,10 @@
         <v>0</v>
       </c>
       <c r="E91" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F91" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>1</v>
@@ -3909,10 +3909,10 @@
         <v>0</v>
       </c>
       <c r="E92" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F92" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>1</v>
@@ -3932,10 +3932,10 @@
         <v>0</v>
       </c>
       <c r="E93" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F93" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>1</v>
@@ -3955,10 +3955,10 @@
         <v>0</v>
       </c>
       <c r="E94" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F94" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>1</v>
@@ -3978,10 +3978,10 @@
         <v>0</v>
       </c>
       <c r="E95" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F95" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>1</v>
@@ -4001,10 +4001,10 @@
         <v>0</v>
       </c>
       <c r="E96" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F96" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>1</v>
@@ -4024,10 +4024,10 @@
         <v>0</v>
       </c>
       <c r="E97" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F97" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>1</v>
@@ -4047,10 +4047,10 @@
         <v>0</v>
       </c>
       <c r="E98" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F98" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>1</v>
@@ -4070,10 +4070,10 @@
         <v>0</v>
       </c>
       <c r="E99" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F99" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>1</v>
@@ -4093,10 +4093,10 @@
         <v>0</v>
       </c>
       <c r="E100" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F100" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>1</v>
@@ -4116,10 +4116,10 @@
         <v>0</v>
       </c>
       <c r="E101" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F101" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>1</v>
@@ -4139,10 +4139,10 @@
         <v>0</v>
       </c>
       <c r="E102" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F102" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>1</v>
@@ -4162,10 +4162,10 @@
         <v>0</v>
       </c>
       <c r="E103" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F103" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>1</v>
@@ -4185,10 +4185,10 @@
         <v>0</v>
       </c>
       <c r="E104" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F104" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>1</v>
@@ -4208,10 +4208,10 @@
         <v>0</v>
       </c>
       <c r="E105" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F105" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>1</v>
@@ -4231,10 +4231,10 @@
         <v>0</v>
       </c>
       <c r="E106" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F106" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>1</v>
@@ -4254,10 +4254,10 @@
         <v>0</v>
       </c>
       <c r="E107" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F107" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>1</v>
@@ -4277,10 +4277,10 @@
         <v>0</v>
       </c>
       <c r="E108" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F108" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>1</v>
@@ -4300,10 +4300,10 @@
         <v>0</v>
       </c>
       <c r="E109" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F109" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>1</v>
@@ -4323,10 +4323,10 @@
         <v>0</v>
       </c>
       <c r="E110" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F110" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G110" s="1" t="s">
         <v>1</v>
@@ -4346,10 +4346,10 @@
         <v>0</v>
       </c>
       <c r="E111" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F111" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>1</v>
@@ -4369,10 +4369,10 @@
         <v>0</v>
       </c>
       <c r="E112" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F112" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>1</v>
@@ -4392,10 +4392,10 @@
         <v>0</v>
       </c>
       <c r="E113" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F113" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>1</v>
@@ -4415,10 +4415,10 @@
         <v>0</v>
       </c>
       <c r="E114" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F114" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G114" s="1" t="s">
         <v>1</v>
@@ -4438,10 +4438,10 @@
         <v>0</v>
       </c>
       <c r="E115" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F115" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>1</v>
@@ -4461,10 +4461,10 @@
         <v>0</v>
       </c>
       <c r="E116" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F116" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G116" s="1" t="s">
         <v>1</v>
@@ -4484,10 +4484,10 @@
         <v>0</v>
       </c>
       <c r="E117" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F117" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>1</v>
@@ -4507,10 +4507,10 @@
         <v>0</v>
       </c>
       <c r="E118" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F118" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G118" s="1" t="s">
         <v>1</v>
@@ -4530,10 +4530,10 @@
         <v>0</v>
       </c>
       <c r="E119" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F119" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>1</v>
@@ -4553,10 +4553,10 @@
         <v>0</v>
       </c>
       <c r="E120" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F120" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G120" s="1" t="s">
         <v>1</v>
@@ -4576,10 +4576,10 @@
         <v>0</v>
       </c>
       <c r="E121" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F121" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>1</v>
@@ -4599,10 +4599,10 @@
         <v>0</v>
       </c>
       <c r="E122" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F122" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>1</v>
@@ -4622,10 +4622,10 @@
         <v>0</v>
       </c>
       <c r="E123" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F123" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>2</v>
@@ -4645,10 +4645,10 @@
         <v>0</v>
       </c>
       <c r="E124" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F124" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>2</v>
@@ -4668,10 +4668,10 @@
         <v>0</v>
       </c>
       <c r="E125" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F125" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>2</v>
@@ -4691,10 +4691,10 @@
         <v>0</v>
       </c>
       <c r="E126" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F126" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>2</v>
@@ -4714,10 +4714,10 @@
         <v>0</v>
       </c>
       <c r="E127" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F127" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>2</v>
@@ -4737,10 +4737,10 @@
         <v>0</v>
       </c>
       <c r="E128" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F128" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>2</v>
@@ -4760,10 +4760,10 @@
         <v>0</v>
       </c>
       <c r="E129" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F129" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>2</v>
@@ -4783,10 +4783,10 @@
         <v>0</v>
       </c>
       <c r="E130" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F130" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>2</v>
@@ -4806,10 +4806,10 @@
         <v>0</v>
       </c>
       <c r="E131" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F131" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>2</v>
@@ -4829,10 +4829,10 @@
         <v>0</v>
       </c>
       <c r="E132" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F132" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>2</v>
@@ -4852,10 +4852,10 @@
         <v>0</v>
       </c>
       <c r="E133" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F133" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>2</v>
@@ -4875,10 +4875,10 @@
         <v>0</v>
       </c>
       <c r="E134" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F134" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>2</v>
@@ -4898,10 +4898,10 @@
         <v>0</v>
       </c>
       <c r="E135" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F135" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>2</v>
@@ -4921,10 +4921,10 @@
         <v>0</v>
       </c>
       <c r="E136" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F136" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>2</v>
@@ -4944,10 +4944,10 @@
         <v>0</v>
       </c>
       <c r="E137" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F137" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G137" s="1" t="s">
         <v>2</v>
@@ -4967,10 +4967,10 @@
         <v>0</v>
       </c>
       <c r="E138" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F138" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G138" s="1" t="s">
         <v>2</v>
@@ -4990,10 +4990,10 @@
         <v>0</v>
       </c>
       <c r="E139" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F139" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G139" s="1" t="s">
         <v>2</v>
@@ -5013,10 +5013,10 @@
         <v>0</v>
       </c>
       <c r="E140" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F140" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G140" s="1" t="s">
         <v>2</v>
@@ -5036,10 +5036,10 @@
         <v>0</v>
       </c>
       <c r="E141" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F141" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>2</v>
@@ -5059,10 +5059,10 @@
         <v>0</v>
       </c>
       <c r="E142" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F142" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G142" s="1" t="s">
         <v>2</v>
@@ -5082,10 +5082,10 @@
         <v>0</v>
       </c>
       <c r="E143" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F143" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G143" s="1" t="s">
         <v>2</v>
@@ -5105,10 +5105,10 @@
         <v>0</v>
       </c>
       <c r="E144" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F144" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G144" s="1" t="s">
         <v>2</v>
@@ -5128,10 +5128,10 @@
         <v>0</v>
       </c>
       <c r="E145" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F145" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G145" s="1" t="s">
         <v>2</v>
@@ -5151,10 +5151,10 @@
         <v>0</v>
       </c>
       <c r="E146" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F146" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G146" s="1" t="s">
         <v>2</v>
@@ -5174,10 +5174,10 @@
         <v>0</v>
       </c>
       <c r="E147" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F147" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>2</v>
@@ -5197,10 +5197,10 @@
         <v>0</v>
       </c>
       <c r="E148" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F148" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>2</v>
@@ -5220,10 +5220,10 @@
         <v>0</v>
       </c>
       <c r="E149" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F149" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G149" s="1" t="s">
         <v>2</v>
@@ -5243,10 +5243,10 @@
         <v>0</v>
       </c>
       <c r="E150" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F150" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>2</v>
@@ -5266,10 +5266,10 @@
         <v>0</v>
       </c>
       <c r="E151" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F151" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G151" s="1" t="s">
         <v>2</v>
@@ -5289,10 +5289,10 @@
         <v>0</v>
       </c>
       <c r="E152" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F152" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>2</v>
@@ -5312,10 +5312,10 @@
         <v>0</v>
       </c>
       <c r="E153" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F153" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G153" s="1" t="s">
         <v>2</v>
@@ -5335,10 +5335,10 @@
         <v>0</v>
       </c>
       <c r="E154" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F154" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>2</v>
@@ -5358,10 +5358,10 @@
         <v>0</v>
       </c>
       <c r="E155" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F155" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>2</v>
@@ -5381,10 +5381,10 @@
         <v>0</v>
       </c>
       <c r="E156" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F156" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G156" s="1" t="s">
         <v>2</v>
@@ -5404,10 +5404,10 @@
         <v>0</v>
       </c>
       <c r="E157" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F157" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G157" s="1" t="s">
         <v>2</v>
@@ -5427,10 +5427,10 @@
         <v>0</v>
       </c>
       <c r="E158" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F158" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G158" s="1" t="s">
         <v>2</v>
@@ -5450,10 +5450,10 @@
         <v>0</v>
       </c>
       <c r="E159" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F159" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G159" s="1" t="s">
         <v>2</v>
@@ -5473,10 +5473,10 @@
         <v>0</v>
       </c>
       <c r="E160" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F160" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G160" s="1" t="s">
         <v>2</v>
@@ -5496,10 +5496,10 @@
         <v>0</v>
       </c>
       <c r="E161" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F161" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G161" s="1" t="s">
         <v>2</v>
@@ -5519,10 +5519,10 @@
         <v>0</v>
       </c>
       <c r="E162" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F162" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G162" s="1" t="s">
         <v>2</v>
@@ -5542,10 +5542,10 @@
         <v>0</v>
       </c>
       <c r="E163" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F163" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G163" s="1" t="s">
         <v>2</v>
@@ -5565,10 +5565,10 @@
         <v>0</v>
       </c>
       <c r="E164" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F164" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G164" s="1" t="s">
         <v>2</v>
@@ -5588,10 +5588,10 @@
         <v>0</v>
       </c>
       <c r="E165" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F165" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G165" s="1" t="s">
         <v>2</v>
@@ -5611,10 +5611,10 @@
         <v>0</v>
       </c>
       <c r="E166" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F166" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G166" s="1" t="s">
         <v>2</v>
@@ -5634,10 +5634,10 @@
         <v>0</v>
       </c>
       <c r="E167" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F167" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G167" s="1" t="s">
         <v>2</v>
@@ -5657,10 +5657,10 @@
         <v>0</v>
       </c>
       <c r="E168" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F168" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G168" s="1" t="s">
         <v>2</v>
@@ -5680,10 +5680,10 @@
         <v>0</v>
       </c>
       <c r="E169" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F169" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G169" s="1" t="s">
         <v>2</v>
@@ -5703,10 +5703,10 @@
         <v>0</v>
       </c>
       <c r="E170" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F170" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G170" s="1" t="s">
         <v>2</v>
@@ -5726,10 +5726,10 @@
         <v>0</v>
       </c>
       <c r="E171" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F171" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G171" s="1" t="s">
         <v>2</v>
@@ -5749,10 +5749,10 @@
         <v>0</v>
       </c>
       <c r="E172" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F172" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G172" s="1" t="s">
         <v>2</v>
@@ -5772,10 +5772,10 @@
         <v>0</v>
       </c>
       <c r="E173" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F173" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G173" s="1" t="s">
         <v>2</v>
@@ -5795,10 +5795,10 @@
         <v>0</v>
       </c>
       <c r="E174" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F174" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G174" s="1" t="s">
         <v>2</v>
@@ -5818,10 +5818,10 @@
         <v>0</v>
       </c>
       <c r="E175" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F175" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G175" s="1" t="s">
         <v>2</v>
@@ -5841,10 +5841,10 @@
         <v>0</v>
       </c>
       <c r="E176" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F176" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G176" s="1" t="s">
         <v>2</v>
@@ -5864,10 +5864,10 @@
         <v>0</v>
       </c>
       <c r="E177" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F177" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G177" s="1" t="s">
         <v>2</v>
@@ -5887,10 +5887,10 @@
         <v>0</v>
       </c>
       <c r="E178" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F178" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G178" s="1" t="s">
         <v>2</v>
@@ -5910,10 +5910,10 @@
         <v>0</v>
       </c>
       <c r="E179" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F179" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G179" s="1" t="s">
         <v>2</v>
@@ -5933,10 +5933,10 @@
         <v>0</v>
       </c>
       <c r="E180" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F180" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G180" s="1" t="s">
         <v>2</v>
@@ -5956,10 +5956,10 @@
         <v>0</v>
       </c>
       <c r="E181" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F181" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G181" s="1" t="s">
         <v>2</v>
@@ -5979,10 +5979,10 @@
         <v>0</v>
       </c>
       <c r="E182" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F182" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G182" s="1" t="s">
         <v>2</v>
@@ -6002,10 +6002,10 @@
         <v>0</v>
       </c>
       <c r="E183" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F183" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G183" s="1" t="s">
         <v>2</v>
@@ -6025,10 +6025,10 @@
         <v>0</v>
       </c>
       <c r="E184" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F184" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G184" s="1" t="s">
         <v>2</v>
@@ -6048,10 +6048,10 @@
         <v>0</v>
       </c>
       <c r="E185" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F185" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G185" s="1" t="s">
         <v>2</v>
@@ -6071,10 +6071,10 @@
         <v>0</v>
       </c>
       <c r="E186" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F186" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G186" s="1" t="s">
         <v>2</v>
@@ -6094,10 +6094,10 @@
         <v>0</v>
       </c>
       <c r="E187" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F187" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G187" s="1" t="s">
         <v>2</v>
@@ -6117,10 +6117,10 @@
         <v>0</v>
       </c>
       <c r="E188" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F188" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G188" s="1" t="s">
         <v>2</v>
@@ -6140,10 +6140,10 @@
         <v>0</v>
       </c>
       <c r="E189" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F189" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G189" s="1" t="s">
         <v>2</v>
@@ -6163,10 +6163,10 @@
         <v>0</v>
       </c>
       <c r="E190" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F190" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G190" s="1" t="s">
         <v>2</v>
@@ -6186,10 +6186,10 @@
         <v>0</v>
       </c>
       <c r="E191" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F191" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G191" s="1" t="s">
         <v>2</v>
@@ -6209,10 +6209,10 @@
         <v>0</v>
       </c>
       <c r="E192" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F192" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G192" s="1" t="s">
         <v>2</v>
@@ -6232,10 +6232,10 @@
         <v>0</v>
       </c>
       <c r="E193" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F193" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G193" s="1" t="s">
         <v>2</v>
@@ -6255,10 +6255,10 @@
         <v>0</v>
       </c>
       <c r="E194" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F194" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G194" s="1" t="s">
         <v>2</v>
@@ -6278,10 +6278,10 @@
         <v>0</v>
       </c>
       <c r="E195" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F195" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G195" s="1" t="s">
         <v>2</v>
@@ -6301,10 +6301,10 @@
         <v>0</v>
       </c>
       <c r="E196" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F196" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G196" s="1" t="s">
         <v>2</v>
@@ -6324,10 +6324,10 @@
         <v>0</v>
       </c>
       <c r="E197" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F197" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G197" s="1" t="s">
         <v>2</v>
@@ -6347,10 +6347,10 @@
         <v>0</v>
       </c>
       <c r="E198" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F198" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G198" s="1" t="s">
         <v>2</v>
@@ -6370,10 +6370,10 @@
         <v>0</v>
       </c>
       <c r="E199" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F199" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G199" s="1" t="s">
         <v>2</v>
@@ -6393,10 +6393,10 @@
         <v>0</v>
       </c>
       <c r="E200" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F200" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G200" s="1" t="s">
         <v>2</v>
@@ -6416,10 +6416,10 @@
         <v>0</v>
       </c>
       <c r="E201" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F201" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G201" s="1" t="s">
         <v>2</v>
@@ -6439,10 +6439,10 @@
         <v>0</v>
       </c>
       <c r="E202" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F202" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G202" s="1" t="s">
         <v>2</v>
@@ -6462,10 +6462,10 @@
         <v>0</v>
       </c>
       <c r="E203" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F203" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G203" s="1" t="s">
         <v>2</v>
@@ -6485,10 +6485,10 @@
         <v>0</v>
       </c>
       <c r="E204" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F204" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G204" s="1" t="s">
         <v>2</v>
@@ -6508,10 +6508,10 @@
         <v>0</v>
       </c>
       <c r="E205" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F205" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G205" s="1" t="s">
         <v>2</v>
@@ -6531,10 +6531,10 @@
         <v>0</v>
       </c>
       <c r="E206" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F206" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G206" s="1" t="s">
         <v>2</v>
@@ -6554,10 +6554,10 @@
         <v>0</v>
       </c>
       <c r="E207" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F207" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G207" s="1" t="s">
         <v>2</v>
@@ -6577,10 +6577,10 @@
         <v>0</v>
       </c>
       <c r="E208" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F208" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G208" s="1" t="s">
         <v>2</v>
@@ -6600,10 +6600,10 @@
         <v>0</v>
       </c>
       <c r="E209" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F209" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G209" s="1" t="s">
         <v>2</v>
@@ -6623,10 +6623,10 @@
         <v>0</v>
       </c>
       <c r="E210" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F210" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G210" s="1" t="s">
         <v>2</v>
@@ -6646,10 +6646,10 @@
         <v>0</v>
       </c>
       <c r="E211" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F211" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G211" s="1" t="s">
         <v>2</v>
@@ -6669,10 +6669,10 @@
         <v>0</v>
       </c>
       <c r="E212" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F212" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G212" s="1" t="s">
         <v>2</v>
@@ -6692,10 +6692,10 @@
         <v>0</v>
       </c>
       <c r="E213" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F213" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G213" s="1" t="s">
         <v>2</v>
@@ -6715,10 +6715,10 @@
         <v>0</v>
       </c>
       <c r="E214" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F214" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G214" s="1" t="s">
         <v>2</v>
@@ -6738,10 +6738,10 @@
         <v>0</v>
       </c>
       <c r="E215" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F215" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G215" s="1" t="s">
         <v>2</v>
@@ -6761,10 +6761,10 @@
         <v>0</v>
       </c>
       <c r="E216" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F216" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G216" s="1" t="s">
         <v>2</v>
@@ -6784,10 +6784,10 @@
         <v>0</v>
       </c>
       <c r="E217" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F217" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G217" s="1" t="s">
         <v>2</v>
@@ -6807,10 +6807,10 @@
         <v>0</v>
       </c>
       <c r="E218" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F218" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G218" s="1" t="s">
         <v>2</v>
@@ -6830,10 +6830,10 @@
         <v>0</v>
       </c>
       <c r="E219" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F219" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G219" s="1" t="s">
         <v>2</v>
@@ -6853,10 +6853,10 @@
         <v>0</v>
       </c>
       <c r="E220" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F220" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G220" s="1" t="s">
         <v>2</v>
@@ -6876,10 +6876,10 @@
         <v>0</v>
       </c>
       <c r="E221" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F221" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G221" s="1" t="s">
         <v>2</v>
@@ -6899,10 +6899,10 @@
         <v>0</v>
       </c>
       <c r="E222" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F222" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G222" s="1" t="s">
         <v>2</v>
@@ -6922,10 +6922,10 @@
         <v>0</v>
       </c>
       <c r="E223" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F223" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G223" s="1" t="s">
         <v>2</v>
@@ -6945,10 +6945,10 @@
         <v>0</v>
       </c>
       <c r="E224" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F224" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G224" s="1" t="s">
         <v>2</v>
@@ -6968,10 +6968,10 @@
         <v>0</v>
       </c>
       <c r="E225" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F225" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G225" s="1" t="s">
         <v>2</v>
@@ -6991,10 +6991,10 @@
         <v>0</v>
       </c>
       <c r="E226" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F226" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G226" s="1" t="s">
         <v>2</v>
@@ -7014,10 +7014,10 @@
         <v>0</v>
       </c>
       <c r="E227" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F227" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G227" s="1" t="s">
         <v>2</v>
@@ -7037,10 +7037,10 @@
         <v>0</v>
       </c>
       <c r="E228" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F228" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G228" s="1" t="s">
         <v>2</v>
@@ -7060,10 +7060,10 @@
         <v>0</v>
       </c>
       <c r="E229" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F229" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G229" s="1" t="s">
         <v>2</v>
@@ -7083,10 +7083,10 @@
         <v>0</v>
       </c>
       <c r="E230" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F230" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G230" s="1" t="s">
         <v>2</v>
@@ -7106,10 +7106,10 @@
         <v>0</v>
       </c>
       <c r="E231" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F231" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G231" s="1" t="s">
         <v>2</v>
@@ -7129,10 +7129,10 @@
         <v>0</v>
       </c>
       <c r="E232" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F232" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G232" s="1" t="s">
         <v>2</v>
@@ -7152,10 +7152,10 @@
         <v>0</v>
       </c>
       <c r="E233" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F233" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G233" s="1" t="s">
         <v>2</v>
@@ -7175,10 +7175,10 @@
         <v>0</v>
       </c>
       <c r="E234" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F234" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G234" s="1" t="s">
         <v>2</v>
@@ -7198,10 +7198,10 @@
         <v>0</v>
       </c>
       <c r="E235" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F235" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G235" s="1" t="s">
         <v>2</v>
@@ -7221,10 +7221,10 @@
         <v>0</v>
       </c>
       <c r="E236" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F236" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G236" s="1" t="s">
         <v>2</v>
@@ -7244,10 +7244,10 @@
         <v>0</v>
       </c>
       <c r="E237" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F237" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G237" s="1" t="s">
         <v>2</v>
@@ -7267,10 +7267,10 @@
         <v>0</v>
       </c>
       <c r="E238" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F238" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G238" s="1" t="s">
         <v>2</v>
@@ -7290,10 +7290,10 @@
         <v>0</v>
       </c>
       <c r="E239" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F239" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G239" s="1" t="s">
         <v>2</v>
@@ -7313,10 +7313,10 @@
         <v>0</v>
       </c>
       <c r="E240" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F240" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G240" s="1" t="s">
         <v>2</v>
@@ -7336,10 +7336,10 @@
         <v>0</v>
       </c>
       <c r="E241" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F241" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G241" s="1" t="s">
         <v>2</v>
@@ -7359,10 +7359,10 @@
         <v>0</v>
       </c>
       <c r="E242" s="1">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F242" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G242" s="1" t="s">
         <v>2</v>
@@ -7377,8 +7377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3974093-5C01-5B43-9FD7-98B98BC44827}">
   <dimension ref="A1:G184"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7424,10 +7424,10 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F2">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
@@ -7447,10 +7447,10 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F3">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
@@ -7470,10 +7470,10 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F4">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G4" t="s">
         <v>2</v>
@@ -7493,10 +7493,10 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F5">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G5" t="s">
         <v>2</v>
@@ -7516,10 +7516,10 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F6">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G6" t="s">
         <v>2</v>
@@ -7539,10 +7539,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F7">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G7" t="s">
         <v>2</v>
@@ -7562,10 +7562,10 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F8">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G8" t="s">
         <v>2</v>
@@ -7585,10 +7585,10 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F9">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G9" t="s">
         <v>2</v>
@@ -7608,10 +7608,10 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F10">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G10" t="s">
         <v>2</v>
@@ -7631,10 +7631,10 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F11">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G11" t="s">
         <v>2</v>
@@ -7654,10 +7654,10 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F12">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G12" t="s">
         <v>2</v>
@@ -7677,10 +7677,10 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F13">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G13" t="s">
         <v>2</v>
@@ -7700,10 +7700,10 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F14">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G14" t="s">
         <v>2</v>
@@ -7723,10 +7723,10 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F15">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G15" t="s">
         <v>2</v>
@@ -7746,10 +7746,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F16">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G16" t="s">
         <v>2</v>
@@ -7769,10 +7769,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F17">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G17" t="s">
         <v>2</v>
@@ -7792,10 +7792,10 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F18">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G18" t="s">
         <v>2</v>
@@ -7815,10 +7815,10 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F19">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G19" t="s">
         <v>2</v>
@@ -7838,10 +7838,10 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F20">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G20" t="s">
         <v>2</v>
@@ -7861,10 +7861,10 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F21">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G21" t="s">
         <v>2</v>
@@ -7884,10 +7884,10 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F22">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G22" t="s">
         <v>2</v>
@@ -7907,10 +7907,10 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F23">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G23" t="s">
         <v>2</v>
@@ -7930,10 +7930,10 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F24">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G24" t="s">
         <v>2</v>
@@ -7953,10 +7953,10 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F25">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G25" t="s">
         <v>2</v>
@@ -7976,10 +7976,10 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F26">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G26" t="s">
         <v>2</v>
@@ -7999,10 +7999,10 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F27">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G27" t="s">
         <v>2</v>
@@ -8022,10 +8022,10 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F28">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G28" t="s">
         <v>2</v>
@@ -8045,10 +8045,10 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F29">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G29" t="s">
         <v>2</v>
@@ -8068,10 +8068,10 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F30">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G30" t="s">
         <v>2</v>
@@ -8091,10 +8091,10 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F31">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G31" t="s">
         <v>2</v>
@@ -8114,10 +8114,10 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F32">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G32" t="s">
         <v>2</v>
@@ -8137,10 +8137,10 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F33">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G33" t="s">
         <v>1</v>
@@ -8160,10 +8160,10 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F34">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G34" t="s">
         <v>1</v>
@@ -8183,10 +8183,10 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F35">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G35" t="s">
         <v>1</v>
@@ -8206,10 +8206,10 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F36">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G36" t="s">
         <v>1</v>
@@ -8229,10 +8229,10 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F37">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G37" t="s">
         <v>1</v>
@@ -8252,10 +8252,10 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F38">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G38" t="s">
         <v>1</v>
@@ -8275,10 +8275,10 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F39">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G39" t="s">
         <v>1</v>
@@ -8298,10 +8298,10 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F40">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G40" t="s">
         <v>1</v>
@@ -8321,10 +8321,10 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F41">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G41" t="s">
         <v>1</v>
@@ -8344,10 +8344,10 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F42">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G42" t="s">
         <v>1</v>
@@ -8367,10 +8367,10 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F43">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G43" t="s">
         <v>1</v>
@@ -8390,10 +8390,10 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F44">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G44" t="s">
         <v>1</v>
@@ -8413,10 +8413,10 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F45">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G45" t="s">
         <v>1</v>
@@ -8436,10 +8436,10 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F46">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G46" t="s">
         <v>1</v>
@@ -8459,10 +8459,10 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F47">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G47" t="s">
         <v>1</v>
@@ -8482,10 +8482,10 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F48">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G48" t="s">
         <v>1</v>
@@ -8505,10 +8505,10 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F49">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G49" t="s">
         <v>1</v>
@@ -8528,10 +8528,10 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F50">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G50" t="s">
         <v>1</v>
@@ -8551,10 +8551,10 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F51">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G51" t="s">
         <v>1</v>
@@ -8574,10 +8574,10 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F52">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G52" t="s">
         <v>1</v>
@@ -8597,10 +8597,10 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F53">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G53" t="s">
         <v>1</v>
@@ -8620,10 +8620,10 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F54">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G54" t="s">
         <v>1</v>
@@ -8643,10 +8643,10 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F55">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G55" t="s">
         <v>1</v>
@@ -8666,10 +8666,10 @@
         <v>0</v>
       </c>
       <c r="E56">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F56">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G56" t="s">
         <v>1</v>
@@ -8689,10 +8689,10 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F57">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G57" t="s">
         <v>1</v>
@@ -8712,10 +8712,10 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F58">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G58" t="s">
         <v>1</v>
@@ -8735,10 +8735,10 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F59">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G59" t="s">
         <v>1</v>
@@ -8758,10 +8758,10 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F60">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G60" t="s">
         <v>1</v>
@@ -8781,10 +8781,10 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F61">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G61" t="s">
         <v>1</v>
@@ -8804,10 +8804,10 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="F62">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="G62" t="s">
         <v>1</v>

</xml_diff>